<commit_message>
correction orthographique dans l'horaire
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/bd1/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B081C1EC-8ADE-0B4B-A58E-26556CAFD379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4218E7-1EF5-A148-9FC2-DC835B28065C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{A6EAA84D-6E98-BB4B-8698-E4F48E48897D}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t xml:space="preserve"> Introduction, Diagramme entité-relation </t>
   </si>
   <si>
-    <t xml:space="preserve"> Créer un BD </t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t xml:space="preserve"> 02 févr </t>
   </si>
   <si>
-    <t xml:space="preserve"> Opérations arithm, chaînes, REGEX </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Atelier 4 - formatif formel </t>
   </si>
   <si>
@@ -306,6 +300,12 @@
   </si>
   <si>
     <t xml:space="preserve"> **TP à remettre cours 27** </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Créer une BD </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Opérations arithmétiques, chaînes, REGEX </t>
   </si>
 </sst>
 </file>
@@ -680,7 +680,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -691,7 +691,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -732,39 +732,39 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -775,48 +775,48 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4">
         <v>1.5</v>
       </c>
       <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>2.1</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -827,48 +827,48 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>2.2000000000000002</v>
       </c>
       <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>23</v>
       </c>
-      <c r="G6" t="s">
-        <v>24</v>
-      </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7">
         <v>2.2999999999999998</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -879,48 +879,48 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8">
         <v>2.4</v>
       </c>
       <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
         <v>29</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>2.5</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -931,48 +931,48 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D10">
         <v>2.5</v>
       </c>
       <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
         <v>33</v>
       </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" t="s">
-        <v>35</v>
-      </c>
       <c r="H10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D11">
         <v>2.6</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -983,48 +983,48 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1035,48 +1035,48 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
         <v>45</v>
       </c>
-      <c r="D15" t="s">
+      <c r="F15" t="s">
         <v>46</v>
       </c>
-      <c r="E15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" t="s">
-        <v>48</v>
-      </c>
       <c r="G15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1087,48 +1087,48 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D16">
         <v>4.0999999999999996</v>
       </c>
       <c r="E16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" t="s">
         <v>50</v>
       </c>
-      <c r="F16" t="s">
-        <v>51</v>
-      </c>
-      <c r="G16" t="s">
-        <v>52</v>
-      </c>
       <c r="H16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D17">
         <v>4.2</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1139,48 +1139,48 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D18">
         <v>4.3</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1191,45 +1191,45 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" t="s">
         <v>59</v>
       </c>
-      <c r="D20" t="s">
+      <c r="F20" t="s">
         <v>60</v>
       </c>
-      <c r="E20" t="s">
+      <c r="G20" t="s">
         <v>61</v>
-      </c>
-      <c r="F20" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1240,48 +1240,48 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D22">
         <v>5.2</v>
       </c>
       <c r="E22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" t="s">
         <v>67</v>
-      </c>
-      <c r="F22" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" t="s">
-        <v>68</v>
-      </c>
-      <c r="H22" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1292,48 +1292,48 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D24">
         <v>5.3</v>
       </c>
       <c r="E24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D25">
         <v>5.3</v>
       </c>
       <c r="E25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1344,45 +1344,45 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27">
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1393,48 +1393,48 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B29">
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1445,48 +1445,48 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31">
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>